<commit_message>
ping and wifi test code
</commit_message>
<xml_diff>
--- a/RoverMain/heading_math.xlsx
+++ b/RoverMain/heading_math.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Senior Design\Tiva Code\RoverMain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Google Drive\Senior Design\Tiva Code\SARSRover\RoverMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -402,19 +402,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>28.582377999999999</v>
+        <v>28.628305000000001</v>
       </c>
       <c r="C2" s="1">
         <f>RADIANS(B2)</f>
-        <v>0.49885660414959176</v>
+        <v>0.49965818151515529</v>
       </c>
       <c r="D2">
         <f>SIN(C2)</f>
-        <v>0.47842180117375477</v>
+        <v>0.47912553666040286</v>
       </c>
       <c r="E2">
         <f>COS(C2)</f>
-        <v>0.87813016128684496</v>
+        <v>0.87774638713006448</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -422,19 +422,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>-81.202979999999997</v>
+        <v>-81.199619999999996</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C5" si="0">RADIANS(B3)</f>
-        <v>-1.417259363431105</v>
+        <v>-1.417200720368238</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D5" si="1">SIN(C3)</f>
-        <v>-0.98823633702743396</v>
+        <v>-0.98822736678432854</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="2">COS(C3)</f>
-        <v>0.15293443751686506</v>
+        <v>0.15299239045950022</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -442,19 +442,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>28.582183000000001</v>
+        <v>28.628391000000001</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>0.49885320075755041</v>
+        <v>0.499659682498312</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>0.47841881254978175</v>
+        <v>0.47912685414240608</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>0.87813178953870974</v>
+        <v>0.8777456679697152</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -462,39 +462,39 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-81.202770000000001</v>
+        <v>-81.200012999999998</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>-1.4172556982396758</v>
+        <v>-1.4172075795121983</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-0.98823577648680661</v>
+        <v>-0.98822841615791257</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>0.15293805959119036</v>
+        <v>0.15298561206212694</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>ATAN2(SIN(C4-C2) * E4, (E2 * E4) -( D2 * D4) * COS(C4-C2))</f>
-        <v>1.5708018385475793</v>
+        <v>1.5707938909666652</v>
       </c>
       <c r="B7">
         <f>ATAN2(F2 * F4 - E2 * E4 * COS(D4-D2), SIN(D4-D2) * F4)</f>
         <v>3.1415926535897931</v>
       </c>
       <c r="D7" s="1">
-        <f>ATAN2(COS(C2) * SIN(C4) - SIN(C2) * COS(C4) * COS(C5-C3), SIN(C5-C3) * COS(C4))</f>
-        <v>2.3841048809442063</v>
+        <f>ATAN2( SIN(C5-C3) * COS(C4), COS(C2) * SIN(C4) - SIN(C2) * COS(C4) * COS(C5-C3))</f>
+        <v>2.8972633076836569</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>DEGREES(A7)</f>
-        <v>90.000315800166433</v>
+        <v>89.999860437322724</v>
       </c>
       <c r="B8">
         <f>DEGREES(B7)</f>
@@ -502,31 +502,31 @@
       </c>
       <c r="D8" s="1">
         <f>DEGREES(D7)</f>
-        <v>136.59914759464263</v>
+        <v>166.0009596683864</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>LN(TAN(B4/2+PI()/4) / TAN(B2/2+PI()/4))</f>
-        <v>2.0462602526706057E-4</v>
+        <v>-9.1685537943557267E-5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>ABS(B3-B5)</f>
-        <v>2.0999999999560259E-4</v>
+        <v>3.9300000000253021E-4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>ATAN2(A11,A10)</f>
-        <v>0.77243787265238284</v>
+        <v>-0.2291970339258238</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>DEGREES(A12)</f>
-        <v>44.257430039045289</v>
+        <v>-13.13202272086645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>